<commit_message>
I literally, rebuilt the whole Controle.py program, restructuring it in class and functions for later optimization and implementation in a GUI app
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +615,26 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B0BF67DM6K</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SteelSeries Apex Pro TKL Wireless HyperMagnetic Gaming Keyboard — World's Fastest Keyboard — Esports Tenkeyless — OLED Screen — Adjustable Actuation — PBT Keycaps — Bluetooth — 2.4GHz — USB-C</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>993.49</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>02/03/2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added comments and TODOs - modified prints
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,6 +635,26 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>B0C9THQ36P</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>XVX Retro 75% Gaming Keyboard with OLED Display&amp;Knob, M87 Pro Bluetooth 5.1/2.4GHz /USB-C Wireless Mechanical Keyboard with Hot-Swappable Custom Switch, Compact TKL Gamer RGB Keyboard, PBT Keycaps</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>392.4</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>02/03/2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>